<commit_message>
Huso horario interaccion espacio colaborativo
</commit_message>
<xml_diff>
--- a/docs/formatos/interaccionColaborativo.xlsx
+++ b/docs/formatos/interaccionColaborativo.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22609"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E79BA18A-C8F5-43C1-9D1F-3A3DB3780DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,21 +13,38 @@
   <definedNames>
     <definedName name="USUARIOS_20150209" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Evaluaciones por módulo. Desde DD/MM/AAAA. Hasta DD/MM/AAAA.</t>
   </si>
   <si>
+    <t xml:space="preserve">Empresa: YYYYYYYYYY. Programa: Pensamiento estratégico. </t>
+  </si>
+  <si>
+    <t>Tema: Espacio</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -36,6 +54,12 @@
     <t>Apellido</t>
   </si>
   <si>
+    <t>Fecha de Registro</t>
+  </si>
+  <si>
+    <t>Hora de Registro</t>
+  </si>
+  <si>
     <t>Correo</t>
   </si>
   <si>
@@ -57,32 +81,20 @@
     <t>Campo4</t>
   </si>
   <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>Fecha de Registro</t>
-  </si>
-  <si>
     <t>Fecha de mensaje</t>
   </si>
   <si>
+    <t>Hora de mensaje</t>
+  </si>
+  <si>
     <t>Mensaje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empresa: YYYYYYYYYY. Programa: Pensamiento estratégico. </t>
-  </si>
-  <si>
-    <t>Tema: Espacio</t>
-  </si>
-  <si>
-    <t>Hora de mensaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,17 +205,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -478,159 +490,166 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="50.140625" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" customWidth="1"/>
+    <col min="16" max="16" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" ht="20.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:16" ht="20.25">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+    </row>
+    <row r="3" spans="1:16" s="11" customFormat="1" ht="20.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
+      <c r="N5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" s="11" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-    </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="35.1" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="8"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="8"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="10"/>
+    <row r="28" spans="7:7">
+      <c r="G28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>